<commit_message>
- Fixed typo issue "Rougelike" to "Roguelike" in project description, project name and banner image.
</commit_message>
<xml_diff>
--- a/tools/projects.xlsx
+++ b/tools/projects.xlsx
@@ -95,6 +95,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">Sharpen your reflexes in this fast-paced, top-down shooter for </t>
     </r>
     <r>
@@ -128,10 +135,10 @@
 1#/images/projects/casual-shooter/cts-enemies.png</t>
   </si>
   <si>
-    <t>Action Rougelike</t>
-  </si>
-  <si>
-    <t>/images/projects/action-rougelike/ar-banner.png</t>
+    <t>Action Roguelike</t>
+  </si>
+  <si>
+    <t>/images/projects/action-roguelike/ar-banner.png</t>
   </si>
   <si>
     <t>2022-2023</t>
@@ -142,11 +149,11 @@
   <si>
     <t>3#https://youtu.be/mfHQZCE7S80
 0#This was my university graduation project in my final year.
-0# What I worked on:\\n- Rougelike combat. \\n- Random rooms and upgrades system. \\n- Enemy AI, trap system. \\n- Save load system.\\n- Event trigger, simple shop.
+0# What I worked on:\\n- Roguelike combat. \\n- Random rooms and upgrades system. \\n- Enemy AI, trap system. \\n- Save load system.\\n- Event trigger, simple shop.
 0# Full gameplay.
 3#https://youtu.be/8IbrqM4H0rg
-1#/images/projects/action-rougelike/ar-combat-2.png
-2#/images/projects/action-rougelike/ar-combat.gif</t>
+1#/images/projects/action-roguelike/ar-combat-2.png
+2#/images/projects/action-roguelike/ar-combat.gif</t>
   </si>
   <si>
     <t>Deverse World</t>
@@ -182,7 +189,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,13 +202,6 @@
       <color rgb="FFF5F5F5"/>
       <name val="Arial"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -664,148 +664,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1164,10 +1164,17 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="5"/>
+  <cols>
+    <col min="1" max="1" width="60.2857142857143" customWidth="1"/>
+    <col min="2" max="2" width="42.1428571428571" customWidth="1"/>
+    <col min="3" max="3" width="44.1428571428571" customWidth="1"/>
+    <col min="4" max="4" width="45.4285714285714" customWidth="1"/>
+    <col min="5" max="5" width="90.7142857142857" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">

</xml_diff>